<commit_message>
JS 8 Tugas 3
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE0BFFF9-427A-4A32-B13C-9A9226BFC2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C5B3C8-336F-4677-B7CA-802698927338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3168" windowWidth="13800" windowHeight="7092" xr2:uid="{197DBFFA-AE45-4346-B06D-1B7E070332D1}"/>
+    <workbookView xWindow="3528" yWindow="3516" windowWidth="13800" windowHeight="7092" xr2:uid="{197DBFFA-AE45-4346-B06D-1B7E070332D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>level</t>
   </si>
@@ -49,25 +49,13 @@
     <t>password</t>
   </si>
   <si>
-    <t>admin0</t>
-  </si>
-  <si>
-    <t>manager0</t>
-  </si>
-  <si>
-    <t>admin00</t>
-  </si>
-  <si>
-    <t>admin000</t>
-  </si>
-  <si>
     <t>admin 01</t>
   </si>
   <si>
-    <t>manager 0</t>
-  </si>
-  <si>
-    <t>admin 00</t>
+    <t>coba-coba</t>
+  </si>
+  <si>
+    <t>athif</t>
   </si>
 </sst>
 </file>
@@ -419,14 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501FD9DC-9183-4E24-8C62-9C3119488D26}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -449,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>12345678</v>
@@ -463,40 +452,12 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
         <v>12345678</v>
       </c>
     </row>

</xml_diff>